<commit_message>
updated file to include new sr requirements
</commit_message>
<xml_diff>
--- a/Rules and Requirements/Requirements.xlsx
+++ b/Rules and Requirements/Requirements.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpa9071/Desktop/Rover_Team/Rover_Team/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wpa9071/Documents/Rover_Embedded/Rules and Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017A36FB-20CB-D24F-91B5-8B1DC45D9B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8967D176-4E68-B24D-8369-00DB512F8C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C6A560F9-8541-4338-A35E-7BFE5C788CE2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{C6A560F9-8541-4338-A35E-7BFE5C788CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t xml:space="preserve">Requirements </t>
   </si>
@@ -178,6 +179,57 @@
   </si>
   <si>
     <t>C4</t>
+  </si>
+  <si>
+    <t>Sample Return Module Requirements</t>
+  </si>
+  <si>
+    <t>The Sample Return Arduino shall manage the operation of the motors</t>
+  </si>
+  <si>
+    <t>The Sample Return Arduino shall manage the operation of the servos</t>
+  </si>
+  <si>
+    <t>The Sample Return Arduino will use a clockspring to connect to the primary module</t>
+  </si>
+  <si>
+    <t>The Sample Return Arduino will use the Sabertooth 2x25 for motor and servo control</t>
+  </si>
+  <si>
+    <t>The Sample Return Arduino will connect to the primary module through I2C</t>
+  </si>
+  <si>
+    <t>The Arduino shall be capable of enabling and disabling the motors</t>
+  </si>
+  <si>
+    <t>The Arduino shall parse packets properly</t>
+  </si>
+  <si>
+    <t>The Arduino shall use two way data communications</t>
+  </si>
+  <si>
+    <t>The Sample Return Arduino must be able to communicate with only the primary module</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>The Arduino will have a scheme to set the primary module to sample retrival mode</t>
+  </si>
+  <si>
+    <t>The Arduino shall turn on or off a motor when a proper packet is sent</t>
+  </si>
+  <si>
+    <t>The Arduino shall be capable of enabling and disabling the servos</t>
+  </si>
+  <si>
+    <t>The Servo shall be programmed to run for a specified distance</t>
+  </si>
+  <si>
+    <t>The servos used will be part number: xxxxxxx</t>
+  </si>
+  <si>
+    <t>The motors used will be part number: xxxxxx</t>
   </si>
 </sst>
 </file>
@@ -552,10 +604,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70758C03-10A5-4606-B0B2-76FD4FF6D514}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -769,4 +822,162 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67660C98-CEF2-F540-B8B0-EC328B4D9BEC}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="67.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>